<commit_message>
Final Update before restructure
This is the final update on the project before I restructure the repository
</commit_message>
<xml_diff>
--- a/NFC uid.xlsx
+++ b/NFC uid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tudublin-my.sharepoint.com/personal/c18423664_mytudublin_ie/Documents/Final Year Proposal/Code Implementation/Final-Year-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8979719-3199-427F-BB47-6E66AA1D6B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{F8979719-3199-427F-BB47-6E66AA1D6B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE396694-3929-49B4-8E62-B806945C9B71}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9012" xr2:uid="{67766E74-0C50-4CDB-AC62-75D9A520C5A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{67766E74-0C50-4CDB-AC62-75D9A520C5A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
   <si>
     <t>uid</t>
   </si>
@@ -66,6 +66,30 @@
   </si>
   <si>
     <t>04694C6A266E81</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>Linked</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -417,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D68206-5A05-4522-8AD8-69E13240FC07}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,59 +452,149 @@
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>